<commit_message>
boekjaar als kalenderjaar compleet
</commit_message>
<xml_diff>
--- a/Avantis/Avantis.xlsx
+++ b/Avantis/Avantis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c741cee80ec8cf3/Financieel/IndexFondsen/KeuzeWelkIndexFonds/OnderzoekPerFonds/Avantis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c741cee80ec8cf3/Financieel/IndexFondsenOnderzoek/KeuzeWelkIndexFonds/OnderzoekPerFonds/Avantis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="656" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6720E0E7-207F-4FF8-8744-5D67703A6A20}"/>
+  <xr:revisionPtr revIDLastSave="658" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B54691F4-74DB-443C-8B02-006D2DA8FF3E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Dividend income (net)</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Avantis International Small Cap Value ETF (AVDV)</t>
+  </si>
+  <si>
+    <t>Bookyear != calender year: august</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -145,7 +148,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -443,7 +446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A50C80A-B9F0-42B2-B14F-324E5B39F7D5}">
   <dimension ref="B2:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -486,6 +491,9 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -615,7 +623,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A598ED46-EEA8-4CD3-B87C-CF32F0FABA87}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -658,6 +668,9 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">

</xml_diff>